<commit_message>
new changes for Test page testcases
</commit_message>
<xml_diff>
--- a/target/test-classes/excel/LoginData.xlsx
+++ b/target/test-classes/excel/LoginData.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D59E3B-7F5F-49D6-B020-D901094153DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E192A2C1-548D-4DAD-B745-F75F3CFF0D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="logedinToDashboard" sheetId="3" r:id="rId2"/>
-    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId3"/>
+    <sheet name="verifyPageTitle" sheetId="4" r:id="rId2"/>
+    <sheet name="verifyManageTestFunctionality" sheetId="5" r:id="rId3"/>
+    <sheet name="verifyTheSearchResultMatching" sheetId="6" r:id="rId4"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId5"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="25">
   <si>
     <t>browserName</t>
   </si>
@@ -78,6 +81,30 @@
   </si>
   <si>
     <t>expectedTitle</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Manage Tests</t>
+  </si>
+  <si>
+    <t>patientName</t>
+  </si>
+  <si>
+    <t>mike</t>
+  </si>
+  <si>
+    <t>Automated User One</t>
+  </si>
+  <si>
+    <t>fdghgfhfdgh</t>
+  </si>
+  <si>
+    <t>expectedResult</t>
+  </si>
+  <si>
+    <t>pankaj</t>
   </si>
 </sst>
 </file>
@@ -114,12 +141,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -130,11 +172,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -512,11 +556,314 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10FC8CB-4A15-426F-8D4E-E74EA2F78C46}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EDB2C186-E58F-4954-BB1C-AB0F52AC67EF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{396F2B2E-2E95-480E-97B5-1B8A9401E5B6}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{733D0C12-BAFA-4BCC-9A43-F2D6AA8878BE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E701CD-DCBD-47C8-8E53-2BD507AD24A1}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2224DC66-53E7-47F2-A863-6D09885A776F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{9D29D226-9C1D-4276-8F6E-99C7A4748692}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{DA31E507-8295-4C4E-929F-C05100603F7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D994E9F-663D-4EE0-8F77-E85A904780AE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{66EBC12D-F400-49D5-BF9E-8DBB2373D11C}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{011F5100-1674-4325-A8C2-3F869D8913DE}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A142440B-CD3D-4642-A7AA-5629C663C4ED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>